<commit_message>
Fully working with proper reward function
</commit_message>
<xml_diff>
--- a/Example-Sample-Resources.xlsx
+++ b/Example-Sample-Resources.xlsx
@@ -5,13 +5,16 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>Table 1</t>
+  </si>
   <si>
     <t>Resource</t>
   </si>
@@ -79,9 +82,9 @@
   </numFmts>
   <fonts count="3">
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="12"/>
@@ -89,7 +92,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -102,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -121,6 +124,96 @@
         <color indexed="9"/>
       </top>
       <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
         <color indexed="9"/>
       </bottom>
       <diagonal/>
@@ -128,30 +221,42 @@
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -170,16 +275,17 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
-    <a:clrScheme name="Office Theme">
+    <a:clrScheme name="Blank">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -187,28 +293,28 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="A7A7A7"/>
+        <a:srgbClr val="5E5E5E"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="535353"/>
+        <a:srgbClr val="D5D5D5"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="00A2FF"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="16E7CF"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="61D836"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="FFD932"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="FF644E"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="FF42A1"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -217,7 +323,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office Theme">
+    <a:fontScheme name="Blank">
       <a:majorFont>
         <a:latin typeface="Helvetica Neue"/>
         <a:ea typeface="Helvetica Neue"/>
@@ -229,7 +335,7 @@
         <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office Theme">
+    <a:fmtScheme name="Blank">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -367,50 +473,47 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:srgbClr val="000000"/>
         </a:solidFill>
         <a:ln w="12700" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:noFill/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica Neue Medium"/>
+            <a:ea typeface="Helvetica Neue Medium"/>
+            <a:cs typeface="Helvetica Neue Medium"/>
+            <a:sym typeface="Helvetica Neue Medium"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -660,10 +763,10 @@
         <a:noFill/>
         <a:ln w="12700" cap="flat">
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -950,11 +1053,11 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -978,10 +1081,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1232,157 +1335,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="10.8516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
+    <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" ht="12.9" customHeight="1">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="B2" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="C2" t="s" s="4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s" s="3">
+    <row r="3" ht="27.9" customHeight="1">
+      <c r="A3" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C3" t="s" s="7">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s" s="3">
+    <row r="4" ht="27.7" customHeight="1">
+      <c r="A4" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="B4" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="C4" t="s" s="10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s" s="3">
+    <row r="5" ht="12.7" customHeight="1">
+      <c r="A5" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B5" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="s" s="10">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6">
+    <row r="6" ht="27.7" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
         <v>0.2</v>
       </c>
-      <c r="C5" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="C6" t="s" s="10">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6">
+    <row r="7" ht="27.7" customHeight="1">
+      <c r="A7" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9">
         <v>0.5</v>
       </c>
-      <c r="C6" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C7" t="s" s="10">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6">
+    <row r="8" ht="42.7" customHeight="1">
+      <c r="A8" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="B8" s="9">
         <v>0.8</v>
       </c>
-      <c r="C7" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="C8" t="s" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6">
+    <row r="9" ht="12.7" customHeight="1">
+      <c r="A9" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9">
         <v>0.5</v>
       </c>
-      <c r="C8" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
+      <c r="C9" t="s" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" t="s" s="2">
+    <row r="10" ht="27.7" customHeight="1">
+      <c r="A10" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="C10" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="B9" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="C9" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
     </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B10" s="6">
+    <row r="11" ht="12.7" customHeight="1">
+      <c r="A11" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B11" s="9">
         <v>0.4</v>
       </c>
-      <c r="C10" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="C11" t="s" s="10">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>